<commit_message>
All data collection complete
</commit_message>
<xml_diff>
--- a/data/suma_hit.xlsx
+++ b/data/suma_hit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Pilot Data/summer_pilot/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFB68873-2D60-B64B-B0E2-783BE6CA22DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03DFC83-0ABD-D947-A5A6-70BBCC380591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15760" xr2:uid="{72066A95-7E11-1642-8DC2-2A01365B60AC}"/>
+    <workbookView xWindow="34500" yWindow="4480" windowWidth="27640" windowHeight="15760" xr2:uid="{72066A95-7E11-1642-8DC2-2A01365B60AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -424,6 +424,9 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>